<commit_message>
changes in lots of files
</commit_message>
<xml_diff>
--- a/QA/testcases/CPR/Provider/Prov_Patient_App_Create_PCase_Positive_Alien_POE1.xlsx
+++ b/QA/testcases/CPR/Provider/Prov_Patient_App_Create_PCase_Positive_Alien_POE1.xlsx
@@ -1330,10 +1330,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1360,11 +1360,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1376,16 +1413,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1400,30 +1443,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1431,7 +1451,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1445,27 +1472,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1481,24 +1496,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1525,13 +1525,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1549,7 +1573,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1561,31 +1669,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1597,7 +1687,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1609,103 +1705,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1758,8 +1758,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1769,7 +1771,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1785,6 +1787,24 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1819,15 +1839,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1842,27 +1853,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1874,130 +1874,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2379,8 +2379,8 @@
   <sheetPr/>
   <dimension ref="A1:H221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="H221" sqref="A2:H221"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="E216" sqref="E216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -2656,7 +2656,7 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -3682,7 +3682,7 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>12</v>
@@ -4124,7 +4124,7 @@
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F79" s="7" t="s">
         <v>12</v>
@@ -4184,7 +4184,7 @@
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
       <c r="E82" s="6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>12</v>
@@ -4328,7 +4328,7 @@
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
       <c r="E89" s="7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F89" s="7" t="s">
         <v>12</v>
@@ -4476,7 +4476,7 @@
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
       <c r="E96" s="6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F96" s="6" t="s">
         <v>12</v>
@@ -4764,7 +4764,7 @@
       <c r="C110" s="6"/>
       <c r="D110" s="6"/>
       <c r="E110" s="6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F110" s="6" t="s">
         <v>12</v>
@@ -5556,7 +5556,7 @@
       <c r="C149" s="7"/>
       <c r="D149" s="7"/>
       <c r="E149" s="7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F149" s="7"/>
       <c r="G149" s="7"/>
@@ -5694,7 +5694,7 @@
       <c r="C156" s="6"/>
       <c r="D156" s="6"/>
       <c r="E156" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F156" s="6"/>
       <c r="G156" s="6"/>
@@ -5776,7 +5776,7 @@
       <c r="C160" s="6"/>
       <c r="D160" s="6"/>
       <c r="E160" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F160" s="6"/>
       <c r="G160" s="6"/>
@@ -5966,7 +5966,7 @@
       <c r="C170" s="6"/>
       <c r="D170" s="6"/>
       <c r="E170" s="6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F170" s="6"/>
       <c r="G170" s="6"/>
@@ -6316,7 +6316,7 @@
       <c r="C188" s="6"/>
       <c r="D188" s="6"/>
       <c r="E188" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F188" s="6"/>
       <c r="G188" s="6"/>
@@ -6760,7 +6760,7 @@
       <c r="C211" s="7"/>
       <c r="D211" s="7"/>
       <c r="E211" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F211" s="7"/>
       <c r="G211" s="7"/>
@@ -6842,7 +6842,7 @@
       <c r="C215" s="7"/>
       <c r="D215" s="7"/>
       <c r="E215" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F215" s="7"/>
       <c r="G215" s="7"/>

</xml_diff>